<commit_message>
Revert "fixing map data"
This reverts commit 655278d8d51b0404dd91e5248adaa3406e33dca5.
</commit_message>
<xml_diff>
--- a/Assets/Maps/map 1.xlsx
+++ b/Assets/Maps/map 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beshe\Documents\GitHub\Trip-Navigator-2D\Assets\Maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beshe\Trip Navigator 2D\Assets\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0BF20F-1EA9-47F3-AFA6-2077ECA46E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4D19D1-FDBE-42EB-96D9-F266B974CFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{571CE9F3-7F1B-4A25-A89A-3D67A6FFCAFD}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:CJ40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="CC10" sqref="CC10"/>
+      <selection activeCell="A23" sqref="A23:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2864,7 +2864,7 @@
         <v>2</v>
       </c>
       <c r="CC9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CD9" s="1">
         <v>0</v>

</xml_diff>